<commit_message>
Montreal agenda, final ballot spreadsheets for SDC, CRD and PRO, updates to ballot tracker tools
</commit_message>
<xml_diff>
--- a/Agendas/201901 San Antonio WGM FHIR Agenda.xlsx
+++ b/Agendas/201901 San Antonio WGM FHIR Agenda.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lloyd\Documents\SVN\FHIR-documents\Agendas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05330038-06AB-4A44-A39F-91024E497901}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C80A710-F602-446F-A93D-1E1F7C120A0E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,13 +17,20 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <fileRecoveryPr autoRecover="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="56">
   <si>
     <t>Mon</t>
   </si>
@@ -189,6 +196,9 @@
   </si>
   <si>
     <t>Clinicians on FHIR</t>
+  </si>
+  <si>
+    <t>Update on FHIRCast</t>
   </si>
 </sst>
 </file>
@@ -626,10 +636,10 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +993,7 @@
       <c r="D22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F22" s="7"/>
@@ -1098,7 +1108,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
@@ -1113,6 +1123,9 @@
       </c>
       <c r="F30" s="8" t="s">
         <v>38</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>